<commit_message>
CE01ISSM Corrected reference designators to coincide with 1100-00006 version 1-27
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_CE01ISSM_00003.xlsx
+++ b/deployment/Omaha_Cal_Info_CE01ISSM_00003.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="27435" yWindow="585" windowWidth="29040" windowHeight="16440" tabRatio="759"/>
+    <workbookView xWindow="27435" yWindow="585" windowWidth="29040" windowHeight="16440" tabRatio="759" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
@@ -266,9 +266,6 @@
   </si>
   <si>
     <t>CC_csv</t>
-  </si>
-  <si>
-    <t>CE01ISSM-MFD37-04-DOSTAD000</t>
   </si>
   <si>
     <t>CE01ISSM-RID16-07-NUTNRB000</t>
@@ -710,6 +707,9 @@
   </si>
   <si>
     <t>OL000198</t>
+  </si>
+  <si>
+    <t>CE01ISSM-MFD37-03-DOSTAD000</t>
   </si>
 </sst>
 </file>
@@ -1929,8 +1929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AML5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1950,7 +1950,7 @@
   <sheetData>
     <row r="1" spans="1:14" s="4" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A1" s="56" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B1" s="56" t="s">
         <v>0</v>
@@ -1986,21 +1986,21 @@
         <v>10</v>
       </c>
       <c r="M1" s="56" t="s">
+        <v>152</v>
+      </c>
+      <c r="N1" s="56" t="s">
         <v>153</v>
-      </c>
-      <c r="N1" s="56" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D2" s="7">
         <v>3</v>
@@ -2015,16 +2015,16 @@
         <v>42284</v>
       </c>
       <c r="H2" s="29" t="s">
+        <v>180</v>
+      </c>
+      <c r="I2" s="29" t="s">
         <v>181</v>
-      </c>
-      <c r="I2" s="29" t="s">
-        <v>182</v>
       </c>
       <c r="J2" s="45">
         <v>25</v>
       </c>
       <c r="K2" s="45" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L2" s="36"/>
       <c r="M2" s="46">
@@ -2052,8 +2052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMM190"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2067,7 +2067,7 @@
     <col min="7" max="7" width="22.28515625" style="8" customWidth="1"/>
     <col min="8" max="8" width="26.140625" style="26" customWidth="1"/>
     <col min="9" max="9" width="21" style="8" customWidth="1"/>
-    <col min="10" max="10" width="27.28515625" style="8" customWidth="1"/>
+    <col min="10" max="10" width="12" style="8" customWidth="1"/>
     <col min="11" max="11" width="15.140625" style="8" customWidth="1"/>
     <col min="12" max="12" width="8.85546875" style="8"/>
     <col min="13" max="13" width="15.85546875" style="8" customWidth="1"/>
@@ -2080,7 +2080,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="55" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C1" s="55" t="s">
         <v>12</v>
@@ -2089,7 +2089,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="55" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F1" s="55" t="s">
         <v>13</v>
@@ -2120,24 +2120,28 @@
         <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D3" s="8">
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G3" s="10"/>
       <c r="H3" s="34"/>
       <c r="I3" s="13" t="s">
-        <v>180</v>
+        <v>179</v>
+      </c>
+      <c r="J3" s="8" t="e">
+        <f>MATCH(A3,K:K,0)</f>
+        <v>#N/A</v>
       </c>
       <c r="K3"/>
       <c r="L3"/>
@@ -4189,19 +4193,19 @@
         <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D5" s="8">
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>19</v>
@@ -5233,19 +5237,19 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D6" s="8">
         <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G6" s="10" t="s">
         <v>20</v>
@@ -7305,19 +7309,19 @@
         <v>53</v>
       </c>
       <c r="B8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D8" s="8">
         <v>3</v>
       </c>
       <c r="E8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G8" s="10" t="s">
         <v>19</v>
@@ -7333,19 +7337,19 @@
         <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D9" s="8">
         <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G9" s="10" t="s">
         <v>20</v>
@@ -7361,19 +7365,19 @@
         <v>53</v>
       </c>
       <c r="B10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D10" s="8">
         <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F10" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G10" s="10" t="s">
         <v>54</v>
@@ -7391,19 +7395,19 @@
         <v>53</v>
       </c>
       <c r="B11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D11" s="8">
         <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G11" s="10" t="s">
         <v>55</v>
@@ -7421,19 +7425,19 @@
         <v>53</v>
       </c>
       <c r="B12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D12" s="8">
         <v>3</v>
       </c>
       <c r="E12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G12" s="10" t="s">
         <v>56</v>
@@ -7451,19 +7455,19 @@
         <v>53</v>
       </c>
       <c r="B13" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D13" s="8">
         <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F13" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G13" s="10" t="s">
         <v>57</v>
@@ -7481,19 +7485,19 @@
         <v>53</v>
       </c>
       <c r="B14" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D14" s="8">
         <v>3</v>
       </c>
       <c r="E14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G14" s="10" t="s">
         <v>58</v>
@@ -7511,19 +7515,19 @@
         <v>53</v>
       </c>
       <c r="B15" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D15" s="8">
         <v>3</v>
       </c>
       <c r="E15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F15" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G15" s="10" t="s">
         <v>59</v>
@@ -7541,19 +7545,19 @@
         <v>53</v>
       </c>
       <c r="B16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D16" s="8">
         <v>3</v>
       </c>
       <c r="E16" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F16" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G16" s="10" t="s">
         <v>60</v>
@@ -7571,19 +7575,19 @@
         <v>53</v>
       </c>
       <c r="B17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D17" s="8">
         <v>3</v>
       </c>
       <c r="E17" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F17" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G17" s="10" t="s">
         <v>61</v>
@@ -7601,19 +7605,19 @@
         <v>53</v>
       </c>
       <c r="B18" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D18" s="8">
         <v>3</v>
       </c>
       <c r="E18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F18" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G18" s="10" t="s">
         <v>62</v>
@@ -7631,19 +7635,19 @@
         <v>53</v>
       </c>
       <c r="B19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D19" s="8">
         <v>3</v>
       </c>
       <c r="E19" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F19" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G19" s="10" t="s">
         <v>63</v>
@@ -7661,19 +7665,19 @@
         <v>53</v>
       </c>
       <c r="B20" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D20" s="8">
         <v>3</v>
       </c>
       <c r="E20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F20" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G20" s="10" t="s">
         <v>64</v>
@@ -7691,19 +7695,19 @@
         <v>53</v>
       </c>
       <c r="B21" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D21" s="8">
         <v>3</v>
       </c>
       <c r="E21" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F21" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G21" s="10" t="s">
         <v>65</v>
@@ -7721,19 +7725,19 @@
         <v>53</v>
       </c>
       <c r="B22" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D22" s="8">
         <v>3</v>
       </c>
       <c r="E22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G22" s="10" t="s">
         <v>66</v>
@@ -7751,19 +7755,19 @@
         <v>53</v>
       </c>
       <c r="B23" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D23" s="8">
         <v>3</v>
       </c>
       <c r="E23" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G23" s="10" t="s">
         <v>67</v>
@@ -7781,19 +7785,19 @@
         <v>53</v>
       </c>
       <c r="B24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D24" s="8">
         <v>3</v>
       </c>
       <c r="E24" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F24" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>68</v>
@@ -7811,19 +7815,19 @@
         <v>53</v>
       </c>
       <c r="B25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D25" s="8">
         <v>3</v>
       </c>
       <c r="E25" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G25" s="10" t="s">
         <v>69</v>
@@ -7841,19 +7845,19 @@
         <v>53</v>
       </c>
       <c r="B26" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D26" s="8">
         <v>3</v>
       </c>
       <c r="E26" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F26" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>70</v>
@@ -7871,19 +7875,19 @@
         <v>53</v>
       </c>
       <c r="B27" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D27" s="8">
         <v>3</v>
       </c>
       <c r="E27" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G27" s="10" t="s">
         <v>71</v>
@@ -7901,19 +7905,19 @@
         <v>53</v>
       </c>
       <c r="B28" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D28" s="8">
         <v>3</v>
       </c>
       <c r="E28" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F28" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G28" s="10" t="s">
         <v>72</v>
@@ -7931,19 +7935,19 @@
         <v>53</v>
       </c>
       <c r="B29" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D29" s="8">
         <v>3</v>
       </c>
       <c r="E29" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F29" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G29" s="10" t="s">
         <v>73</v>
@@ -7961,19 +7965,19 @@
         <v>53</v>
       </c>
       <c r="B30" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D30" s="8">
         <v>3</v>
       </c>
       <c r="E30" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F30" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G30" s="10" t="s">
         <v>74</v>
@@ -7991,19 +7995,19 @@
         <v>53</v>
       </c>
       <c r="B31" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D31" s="8">
         <v>3</v>
       </c>
       <c r="E31" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F31" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G31" s="10" t="s">
         <v>75</v>
@@ -8014,6 +8018,7 @@
       <c r="I31"/>
       <c r="J31" s="10"/>
       <c r="K31" s="39"/>
+      <c r="N31" s="10"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32"/>
@@ -8032,16 +8037,16 @@
         <v>77</v>
       </c>
       <c r="B33" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D33" s="8">
         <v>3</v>
       </c>
       <c r="E33" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F33" s="28">
         <v>136</v>
@@ -8060,16 +8065,16 @@
         <v>77</v>
       </c>
       <c r="B34" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D34" s="8">
         <v>3</v>
       </c>
       <c r="E34" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F34" s="28">
         <v>136</v>
@@ -8088,16 +8093,16 @@
         <v>77</v>
       </c>
       <c r="B35" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D35" s="8">
         <v>3</v>
       </c>
       <c r="E35" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F35" s="28">
         <v>136</v>
@@ -8106,7 +8111,7 @@
         <v>78</v>
       </c>
       <c r="H35" s="40" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I35"/>
       <c r="J35" s="10"/>
@@ -8128,28 +8133,28 @@
         <v>77</v>
       </c>
       <c r="B36" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D36" s="10">
         <v>3</v>
       </c>
       <c r="E36" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F36" s="23">
         <v>136</v>
       </c>
       <c r="G36" s="23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H36" s="23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I36" s="23" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J36" s="10"/>
       <c r="K36" s="10"/>
@@ -9187,16 +9192,16 @@
         <v>52</v>
       </c>
       <c r="B38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D38" s="8">
         <v>3</v>
       </c>
       <c r="E38" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F38" s="28">
         <v>995</v>
@@ -9215,16 +9220,16 @@
         <v>52</v>
       </c>
       <c r="B39" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D39" s="8">
         <v>3</v>
       </c>
       <c r="E39" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F39" s="28">
         <v>995</v>
@@ -9243,16 +9248,16 @@
         <v>52</v>
       </c>
       <c r="B40" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D40" s="8">
         <v>3</v>
       </c>
       <c r="E40" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F40" s="28">
         <v>995</v>
@@ -9271,16 +9276,16 @@
         <v>52</v>
       </c>
       <c r="B41" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D41" s="8">
         <v>3</v>
       </c>
       <c r="E41" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F41" s="28">
         <v>995</v>
@@ -9299,16 +9304,16 @@
         <v>52</v>
       </c>
       <c r="B42" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D42" s="8">
         <v>3</v>
       </c>
       <c r="E42" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F42" s="28">
         <v>995</v>
@@ -9327,16 +9332,16 @@
         <v>52</v>
       </c>
       <c r="B43" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D43" s="8">
         <v>3</v>
       </c>
       <c r="E43" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F43" s="28">
         <v>995</v>
@@ -9355,16 +9360,16 @@
         <v>52</v>
       </c>
       <c r="B44" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D44" s="8">
         <v>3</v>
       </c>
       <c r="E44" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F44" s="28">
         <v>995</v>
@@ -9376,7 +9381,7 @@
         <v>124</v>
       </c>
       <c r="I44" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J44" s="10"/>
     </row>
@@ -9385,16 +9390,16 @@
         <v>52</v>
       </c>
       <c r="B45" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D45" s="8">
         <v>3</v>
       </c>
       <c r="E45" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F45" s="28">
         <v>995</v>
@@ -9415,16 +9420,16 @@
         <v>52</v>
       </c>
       <c r="B46" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D46" s="8">
         <v>3</v>
       </c>
       <c r="E46" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F46" s="28">
         <v>995</v>
@@ -9436,7 +9441,7 @@
         <v>1.0760000000000001</v>
       </c>
       <c r="I46" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J46" s="10"/>
     </row>
@@ -9445,16 +9450,16 @@
         <v>52</v>
       </c>
       <c r="B47" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D47" s="8">
         <v>3</v>
       </c>
       <c r="E47" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F47" s="28">
         <v>995</v>
@@ -9484,25 +9489,25 @@
     </row>
     <row r="49" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B49" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D49" s="8">
         <v>3</v>
       </c>
       <c r="E49" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F49" s="28">
         <v>264</v>
       </c>
       <c r="G49" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H49" s="51">
         <v>217</v>
@@ -9515,25 +9520,25 @@
     </row>
     <row r="50" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B50" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D50" s="8">
         <v>3</v>
       </c>
       <c r="E50" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F50" s="28">
         <v>264</v>
       </c>
       <c r="G50" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H50" s="51">
         <v>240</v>
@@ -9546,25 +9551,25 @@
     </row>
     <row r="51" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B51" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D51" s="8">
         <v>3</v>
       </c>
       <c r="E51" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F51" s="28">
         <v>264</v>
       </c>
       <c r="G51" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H51" s="51">
         <v>20.07</v>
@@ -9575,28 +9580,28 @@
     </row>
     <row r="52" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B52" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D52" s="8">
         <v>3</v>
       </c>
       <c r="E52" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F52" s="28">
         <v>264</v>
       </c>
       <c r="G52" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H52" s="51" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I52"/>
       <c r="J52" s="10"/>
@@ -9604,28 +9609,28 @@
     </row>
     <row r="53" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B53" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D53" s="8">
         <v>3</v>
       </c>
       <c r="E53" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F53" s="28">
         <v>264</v>
       </c>
       <c r="G53" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H53" s="51" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I53"/>
       <c r="J53" s="10"/>
@@ -9633,28 +9638,28 @@
     </row>
     <row r="54" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B54" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D54" s="8">
         <v>3</v>
       </c>
       <c r="E54" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F54" s="28">
         <v>264</v>
       </c>
       <c r="G54" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H54" s="51" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I54"/>
       <c r="J54" s="10"/>
@@ -9662,28 +9667,28 @@
     </row>
     <row r="55" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B55" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D55" s="8">
         <v>3</v>
       </c>
       <c r="E55" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F55" s="28">
         <v>264</v>
       </c>
       <c r="G55" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H55" s="51" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I55"/>
       <c r="J55" s="10"/>
@@ -9706,25 +9711,25 @@
         <v>32</v>
       </c>
       <c r="B57" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D57" s="8">
         <v>3</v>
       </c>
       <c r="E57" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F57" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G57" s="10" t="s">
         <v>33</v>
       </c>
       <c r="H57" s="52" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I57"/>
       <c r="J57" s="10"/>
@@ -10750,25 +10755,25 @@
         <v>32</v>
       </c>
       <c r="B58" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D58" s="8">
         <v>3</v>
       </c>
       <c r="E58" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F58" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G58" s="10" t="s">
         <v>34</v>
       </c>
       <c r="H58" s="52" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I58"/>
       <c r="J58" s="10"/>
@@ -11794,19 +11799,19 @@
         <v>32</v>
       </c>
       <c r="B59" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D59" s="8">
         <v>3</v>
       </c>
       <c r="E59" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F59" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G59" s="10" t="s">
         <v>35</v>
@@ -12838,25 +12843,25 @@
         <v>32</v>
       </c>
       <c r="B60" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D60" s="8">
         <v>3</v>
       </c>
       <c r="E60" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F60" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G60" s="10" t="s">
         <v>36</v>
       </c>
       <c r="H60" s="52" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I60"/>
       <c r="J60" s="10"/>
@@ -13882,25 +13887,25 @@
         <v>32</v>
       </c>
       <c r="B61" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D61" s="8">
         <v>3</v>
       </c>
       <c r="E61" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F61" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G61" s="10" t="s">
         <v>37</v>
       </c>
       <c r="H61" s="52" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I61"/>
       <c r="J61" s="10"/>
@@ -14926,25 +14931,25 @@
         <v>32</v>
       </c>
       <c r="B62" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D62" s="8">
         <v>3</v>
       </c>
       <c r="E62" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F62" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G62" s="10" t="s">
         <v>38</v>
       </c>
       <c r="H62" s="52" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I62"/>
       <c r="J62" s="10"/>
@@ -15970,25 +15975,25 @@
         <v>32</v>
       </c>
       <c r="B63" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D63" s="8">
         <v>3</v>
       </c>
       <c r="E63" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F63" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G63" s="10" t="s">
         <v>39</v>
       </c>
       <c r="H63" s="40" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I63"/>
       <c r="J63" s="10"/>
@@ -17014,25 +17019,25 @@
         <v>32</v>
       </c>
       <c r="B64" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D64" s="11">
         <v>3</v>
       </c>
       <c r="E64" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F64" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G64" s="12" t="s">
         <v>40</v>
       </c>
       <c r="H64" s="53" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J64" s="10"/>
     </row>
@@ -17050,25 +17055,25 @@
     </row>
     <row r="66" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B66" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D66" s="8">
         <v>3</v>
       </c>
       <c r="E66" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F66" s="28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G66" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H66" s="40">
         <v>-9.5600000000000004E-2</v>
@@ -17078,25 +17083,25 @@
     </row>
     <row r="67" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A67" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B67" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D67" s="8">
         <v>3</v>
       </c>
       <c r="E67" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F67" s="28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G67" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H67" s="40">
         <v>1.2159</v>
@@ -17106,25 +17111,25 @@
     </row>
     <row r="68" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A68" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B68" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D68" s="8">
         <v>3</v>
       </c>
       <c r="E68" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F68" s="28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G68" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H68" s="40">
         <v>-2.2898999999999998</v>
@@ -17134,25 +17139,25 @@
     </row>
     <row r="69" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A69" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B69" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D69" s="8">
         <v>3</v>
       </c>
       <c r="E69" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F69" s="28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G69" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H69" s="40">
         <v>14.6716</v>
@@ -17162,22 +17167,22 @@
     </row>
     <row r="70" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A70" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B70" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D70" s="8">
         <v>3</v>
       </c>
       <c r="E70" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F70" s="28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G70" s="10" t="s">
         <v>23</v>
@@ -17186,60 +17191,60 @@
         <v>19706</v>
       </c>
       <c r="I70" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J70" s="10"/>
       <c r="AMM70"/>
     </row>
     <row r="71" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A71" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B71" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D71" s="8">
         <v>3</v>
       </c>
       <c r="E71" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F71" s="28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G71" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H71" s="35">
         <v>34</v>
       </c>
       <c r="I71" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J71" s="10"/>
       <c r="AMM71"/>
     </row>
     <row r="72" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A72" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B72" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D72" s="8">
         <v>3</v>
       </c>
       <c r="E72" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F72" s="28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G72" s="10" t="s">
         <v>25</v>
@@ -17253,25 +17258,25 @@
     </row>
     <row r="73" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A73" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B73" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D73" s="8">
         <v>3</v>
       </c>
       <c r="E73" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F73" s="28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G73" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H73" s="35">
         <v>44327</v>
@@ -17297,19 +17302,19 @@
         <v>22</v>
       </c>
       <c r="B75" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D75" s="8">
         <v>3</v>
       </c>
       <c r="E75" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F75" s="28" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G75" s="10" t="s">
         <v>23</v>
@@ -18340,19 +18345,19 @@
         <v>22</v>
       </c>
       <c r="B76" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D76" s="8">
         <v>3</v>
       </c>
       <c r="E76" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F76" s="28" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G76" s="10" t="s">
         <v>24</v>
@@ -19383,19 +19388,19 @@
         <v>22</v>
       </c>
       <c r="B77" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C77" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D77" s="8">
         <v>3</v>
       </c>
       <c r="E77" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F77" s="28" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G77" s="10" t="s">
         <v>25</v>
@@ -20426,19 +20431,19 @@
         <v>22</v>
       </c>
       <c r="B78" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D78" s="8">
         <v>3</v>
       </c>
       <c r="E78" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F78" s="28" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G78" s="10" t="s">
         <v>26</v>
@@ -21469,19 +21474,19 @@
         <v>22</v>
       </c>
       <c r="B79" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D79" s="8">
         <v>3</v>
       </c>
       <c r="E79" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F79" s="28" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G79" s="10" t="s">
         <v>27</v>
@@ -22513,19 +22518,19 @@
         <v>22</v>
       </c>
       <c r="B80" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D80" s="8">
         <v>3</v>
       </c>
       <c r="E80" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F80" s="28" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G80" s="10" t="s">
         <v>28</v>
@@ -23557,19 +23562,19 @@
         <v>22</v>
       </c>
       <c r="B81" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C81" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D81" s="14">
         <v>3</v>
       </c>
       <c r="E81" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F81" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G81" s="14" t="s">
         <v>29</v>
@@ -23578,7 +23583,7 @@
         <v>35</v>
       </c>
       <c r="I81" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J81" s="10"/>
       <c r="K81"/>
@@ -25628,84 +25633,84 @@
     </row>
     <row r="83" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A83" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B83" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D83" s="8">
         <v>3</v>
       </c>
       <c r="E83" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F83" s="28">
         <v>231</v>
       </c>
       <c r="G83" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H83" s="49" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I83"/>
       <c r="J83" s="10"/>
     </row>
     <row r="84" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A84" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B84" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D84" s="8">
         <v>3</v>
       </c>
       <c r="E84" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F84" s="28">
         <v>231</v>
       </c>
       <c r="G84" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H84" s="49" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I84"/>
       <c r="J84" s="10"/>
     </row>
     <row r="85" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A85" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B85" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C85" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D85" s="8">
         <v>3</v>
       </c>
       <c r="E85" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F85" s="28">
         <v>231</v>
       </c>
       <c r="G85" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H85" s="49" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I85"/>
       <c r="J85" s="10"/>
@@ -25727,19 +25732,19 @@
         <v>21</v>
       </c>
       <c r="B87" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D87" s="8">
         <v>3</v>
       </c>
       <c r="E87" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F87" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G87" s="10" t="s">
         <v>19</v>
@@ -26771,19 +26776,19 @@
         <v>21</v>
       </c>
       <c r="B88" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C88" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D88" s="8">
         <v>3</v>
       </c>
       <c r="E88" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F88" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G88" s="10" t="s">
         <v>20</v>
@@ -28840,49 +28845,49 @@
     </row>
     <row r="90" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A90" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B90" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D90" s="8">
         <v>3</v>
       </c>
       <c r="E90" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F90" s="28">
         <v>21524</v>
       </c>
       <c r="G90" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H90" s="25">
         <v>25000</v>
       </c>
       <c r="I90" s="14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J90" s="10"/>
     </row>
     <row r="91" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A91" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B91" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D91" s="8">
         <v>3</v>
       </c>
       <c r="E91" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F91" s="28">
         <v>21524</v>
@@ -28898,19 +28903,19 @@
     </row>
     <row r="92" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A92" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D92" s="8">
         <v>3</v>
       </c>
       <c r="E92" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F92" s="28">
         <v>21524</v>
@@ -28926,25 +28931,25 @@
     </row>
     <row r="93" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A93" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B93" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D93" s="8">
         <v>3</v>
       </c>
       <c r="E93" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F93" s="28">
         <v>21524</v>
       </c>
       <c r="G93" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H93" s="40">
         <v>0.45</v>
@@ -28954,25 +28959,25 @@
     </row>
     <row r="94" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A94" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B94" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D94" s="8">
         <v>3</v>
       </c>
       <c r="E94" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F94" s="28">
         <v>21524</v>
       </c>
       <c r="G94" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H94" s="40">
         <v>0.45</v>
@@ -28982,25 +28987,25 @@
     </row>
     <row r="95" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A95" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B95" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D95" s="8">
         <v>3</v>
       </c>
       <c r="E95" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F95" s="28">
         <v>21524</v>
       </c>
       <c r="G95" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H95" s="40">
         <v>0.45</v>
@@ -29010,25 +29015,25 @@
     </row>
     <row r="96" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A96" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B96" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D96" s="8">
         <v>3</v>
       </c>
       <c r="E96" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F96" s="28">
         <v>21524</v>
       </c>
       <c r="G96" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H96" s="40">
         <v>0.45</v>
@@ -29050,22 +29055,22 @@
     </row>
     <row r="98" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A98" s="23" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B98" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C98" s="33" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D98" s="19">
         <v>3</v>
       </c>
       <c r="E98" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F98" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G98" s="19"/>
       <c r="H98" s="23"/>
@@ -31125,19 +31130,19 @@
         <v>76</v>
       </c>
       <c r="B100" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C100" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D100" s="8">
         <v>3</v>
       </c>
       <c r="E100" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F100" s="28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G100" s="10" t="s">
         <v>19</v>
@@ -31153,19 +31158,19 @@
         <v>76</v>
       </c>
       <c r="B101" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C101" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D101" s="8">
         <v>3</v>
       </c>
       <c r="E101" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F101" s="28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G101" s="10" t="s">
         <v>20</v>
@@ -31181,19 +31186,19 @@
         <v>76</v>
       </c>
       <c r="B102" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C102" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D102" s="8">
         <v>3</v>
       </c>
       <c r="E102" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F102" s="28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G102" s="10" t="s">
         <v>54</v>
@@ -31209,19 +31214,19 @@
         <v>76</v>
       </c>
       <c r="B103" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C103" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D103" s="8">
         <v>3</v>
       </c>
       <c r="E103" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F103" s="28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G103" s="10" t="s">
         <v>55</v>
@@ -31237,19 +31242,19 @@
         <v>76</v>
       </c>
       <c r="B104" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C104" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D104" s="8">
         <v>3</v>
       </c>
       <c r="E104" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F104" s="28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G104" s="10" t="s">
         <v>56</v>
@@ -31265,19 +31270,19 @@
         <v>76</v>
       </c>
       <c r="B105" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C105" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D105" s="8">
         <v>3</v>
       </c>
       <c r="E105" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F105" s="28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G105" s="10" t="s">
         <v>57</v>
@@ -31293,19 +31298,19 @@
         <v>76</v>
       </c>
       <c r="B106" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C106" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D106" s="8">
         <v>3</v>
       </c>
       <c r="E106" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F106" s="28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G106" s="10" t="s">
         <v>58</v>
@@ -31321,19 +31326,19 @@
         <v>76</v>
       </c>
       <c r="B107" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C107" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D107" s="8">
         <v>3</v>
       </c>
       <c r="E107" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F107" s="28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G107" s="10" t="s">
         <v>59</v>
@@ -31349,19 +31354,19 @@
         <v>76</v>
       </c>
       <c r="B108" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C108" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D108" s="8">
         <v>3</v>
       </c>
       <c r="E108" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F108" s="28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G108" s="10" t="s">
         <v>60</v>
@@ -31377,19 +31382,19 @@
         <v>76</v>
       </c>
       <c r="B109" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C109" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D109" s="8">
         <v>3</v>
       </c>
       <c r="E109" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F109" s="28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G109" s="10" t="s">
         <v>61</v>
@@ -31405,19 +31410,19 @@
         <v>76</v>
       </c>
       <c r="B110" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D110" s="8">
         <v>3</v>
       </c>
       <c r="E110" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F110" s="28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G110" s="10" t="s">
         <v>62</v>
@@ -31433,19 +31438,19 @@
         <v>76</v>
       </c>
       <c r="B111" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C111" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D111" s="8">
         <v>3</v>
       </c>
       <c r="E111" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F111" s="28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G111" s="10" t="s">
         <v>63</v>
@@ -31461,19 +31466,19 @@
         <v>76</v>
       </c>
       <c r="B112" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D112" s="8">
         <v>3</v>
       </c>
       <c r="E112" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F112" s="28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G112" s="10" t="s">
         <v>64</v>
@@ -31489,19 +31494,19 @@
         <v>76</v>
       </c>
       <c r="B113" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C113" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D113" s="8">
         <v>3</v>
       </c>
       <c r="E113" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F113" s="28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G113" s="10" t="s">
         <v>65</v>
@@ -31517,19 +31522,19 @@
         <v>76</v>
       </c>
       <c r="B114" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C114" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D114" s="8">
         <v>3</v>
       </c>
       <c r="E114" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F114" s="28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G114" s="10" t="s">
         <v>66</v>
@@ -31545,19 +31550,19 @@
         <v>76</v>
       </c>
       <c r="B115" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C115" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D115" s="8">
         <v>3</v>
       </c>
       <c r="E115" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F115" s="28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G115" s="10" t="s">
         <v>67</v>
@@ -31573,19 +31578,19 @@
         <v>76</v>
       </c>
       <c r="B116" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C116" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D116" s="8">
         <v>3</v>
       </c>
       <c r="E116" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F116" s="28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G116" s="10" t="s">
         <v>68</v>
@@ -31601,19 +31606,19 @@
         <v>76</v>
       </c>
       <c r="B117" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C117" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D117" s="8">
         <v>3</v>
       </c>
       <c r="E117" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F117" s="28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G117" s="10" t="s">
         <v>69</v>
@@ -31629,19 +31634,19 @@
         <v>76</v>
       </c>
       <c r="B118" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C118" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D118" s="8">
         <v>3</v>
       </c>
       <c r="E118" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F118" s="28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G118" s="10" t="s">
         <v>70</v>
@@ -31657,19 +31662,19 @@
         <v>76</v>
       </c>
       <c r="B119" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C119" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D119" s="8">
         <v>3</v>
       </c>
       <c r="E119" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F119" s="28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G119" s="10" t="s">
         <v>71</v>
@@ -31685,19 +31690,19 @@
         <v>76</v>
       </c>
       <c r="B120" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C120" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D120" s="8">
         <v>3</v>
       </c>
       <c r="E120" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F120" s="28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G120" s="10" t="s">
         <v>72</v>
@@ -31713,19 +31718,19 @@
         <v>76</v>
       </c>
       <c r="B121" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C121" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D121" s="8">
         <v>3</v>
       </c>
       <c r="E121" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F121" s="28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G121" s="10" t="s">
         <v>73</v>
@@ -31741,19 +31746,19 @@
         <v>76</v>
       </c>
       <c r="B122" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C122" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D122" s="8">
         <v>3</v>
       </c>
       <c r="E122" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F122" s="28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G122" s="10" t="s">
         <v>74</v>
@@ -31769,19 +31774,19 @@
         <v>76</v>
       </c>
       <c r="B123" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C123" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D123" s="8">
         <v>3</v>
       </c>
       <c r="E123" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F123" s="28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G123" s="10" t="s">
         <v>75</v>
@@ -31806,19 +31811,19 @@
     </row>
     <row r="125" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A125" s="8" t="s">
-        <v>79</v>
+        <v>226</v>
       </c>
       <c r="B125" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C125" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D125" s="8">
         <v>3</v>
       </c>
       <c r="E125" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F125" s="28">
         <v>315</v>
@@ -31833,20 +31838,20 @@
       <c r="J125" s="10"/>
     </row>
     <row r="126" spans="1:1027" x14ac:dyDescent="0.25">
-      <c r="A126" s="8" t="s">
-        <v>79</v>
+      <c r="A126" s="10" t="s">
+        <v>226</v>
       </c>
       <c r="B126" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C126" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D126" s="8">
         <v>3</v>
       </c>
       <c r="E126" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F126" s="28">
         <v>315</v>
@@ -31861,20 +31866,20 @@
       <c r="J126" s="10"/>
     </row>
     <row r="127" spans="1:1027" x14ac:dyDescent="0.25">
-      <c r="A127" s="8" t="s">
-        <v>79</v>
+      <c r="A127" s="10" t="s">
+        <v>226</v>
       </c>
       <c r="B127" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C127" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D127" s="8">
         <v>3</v>
       </c>
       <c r="E127" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F127" s="28">
         <v>315</v>
@@ -31883,38 +31888,38 @@
         <v>78</v>
       </c>
       <c r="H127" s="40" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I127"/>
       <c r="J127" s="10"/>
     </row>
     <row r="128" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A128" s="10" t="s">
-        <v>79</v>
+        <v>226</v>
       </c>
       <c r="B128" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C128" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D128" s="10">
         <v>3</v>
       </c>
       <c r="E128" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F128" s="28">
         <v>315</v>
       </c>
       <c r="G128" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="H128" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="I128" s="23" t="s">
         <v>137</v>
-      </c>
-      <c r="H128" s="23" t="s">
-        <v>170</v>
-      </c>
-      <c r="I128" s="23" t="s">
-        <v>138</v>
       </c>
       <c r="J128" s="10"/>
       <c r="K128" s="10"/>
@@ -32952,25 +32957,25 @@
         <v>41</v>
       </c>
       <c r="B130" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C130" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D130" s="8">
         <v>3</v>
       </c>
       <c r="E130" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F130" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G130" s="10" t="s">
         <v>33</v>
       </c>
       <c r="H130" s="40" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I130"/>
       <c r="J130" s="10"/>
@@ -32980,25 +32985,25 @@
         <v>41</v>
       </c>
       <c r="B131" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C131" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D131" s="8">
         <v>3</v>
       </c>
       <c r="E131" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F131" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G131" s="10" t="s">
         <v>34</v>
       </c>
       <c r="H131" s="40" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I131"/>
       <c r="J131" s="10"/>
@@ -33008,19 +33013,19 @@
         <v>41</v>
       </c>
       <c r="B132" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C132" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D132" s="8">
         <v>3</v>
       </c>
       <c r="E132" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F132" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G132" s="10" t="s">
         <v>35</v>
@@ -33036,25 +33041,25 @@
         <v>41</v>
       </c>
       <c r="B133" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C133" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D133" s="8">
         <v>3</v>
       </c>
       <c r="E133" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F133" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G133" s="10" t="s">
         <v>36</v>
       </c>
       <c r="H133" s="40" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I133"/>
       <c r="J133" s="10"/>
@@ -33064,25 +33069,25 @@
         <v>41</v>
       </c>
       <c r="B134" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C134" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D134" s="8">
         <v>3</v>
       </c>
       <c r="E134" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F134" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G134" s="10" t="s">
         <v>37</v>
       </c>
       <c r="H134" s="40" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I134"/>
       <c r="J134" s="10"/>
@@ -33092,25 +33097,25 @@
         <v>41</v>
       </c>
       <c r="B135" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C135" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D135" s="8">
         <v>3</v>
       </c>
       <c r="E135" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F135" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G135" s="10" t="s">
         <v>38</v>
       </c>
       <c r="H135" s="40" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I135"/>
       <c r="J135" s="10"/>
@@ -33120,25 +33125,25 @@
         <v>41</v>
       </c>
       <c r="B136" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C136" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D136" s="8">
         <v>3</v>
       </c>
       <c r="E136" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F136" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G136" s="10" t="s">
         <v>39</v>
       </c>
       <c r="H136" s="40" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I136"/>
       <c r="J136" s="10"/>
@@ -33148,25 +33153,25 @@
         <v>41</v>
       </c>
       <c r="B137" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C137" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D137" s="8">
         <v>3</v>
       </c>
       <c r="E137" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F137" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G137" s="10" t="s">
         <v>40</v>
       </c>
       <c r="H137" s="40" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I137"/>
       <c r="J137" s="10"/>
@@ -33185,25 +33190,25 @@
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B139" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C139" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D139" s="8">
         <v>3</v>
       </c>
       <c r="E139" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F139" s="29" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G139" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H139" s="40">
         <v>-2.6800000000000001E-2</v>
@@ -33212,25 +33217,25 @@
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B140" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C140" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D140" s="8">
         <v>3</v>
       </c>
       <c r="E140" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F140" s="29" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G140" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H140" s="40">
         <v>0.95989999999999998</v>
@@ -33239,25 +33244,25 @@
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B141" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C141" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D141" s="8">
         <v>3</v>
       </c>
       <c r="E141" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F141" s="29" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G141" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H141" s="40">
         <v>-1.9703999999999999</v>
@@ -33266,25 +33271,25 @@
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B142" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C142" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D142" s="8">
         <v>3</v>
       </c>
       <c r="E142" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F142" s="29" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G142" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H142" s="40">
         <v>16.39</v>
@@ -33293,22 +33298,22 @@
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B143" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C143" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D143" s="8">
         <v>3</v>
       </c>
       <c r="E143" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F143" s="29" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G143" s="10" t="s">
         <v>23</v>
@@ -33320,25 +33325,25 @@
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B144" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C144" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D144" s="8">
         <v>3</v>
       </c>
       <c r="E144" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F144" s="29" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G144" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H144" s="40">
         <v>34</v>
@@ -33347,22 +33352,22 @@
     </row>
     <row r="145" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A145" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B145" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C145" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D145" s="8">
         <v>3</v>
       </c>
       <c r="E145" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F145" s="29" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G145" s="10" t="s">
         <v>25</v>
@@ -33374,25 +33379,25 @@
     </row>
     <row r="146" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A146" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B146" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C146" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D146" s="8">
         <v>3</v>
       </c>
       <c r="E146" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F146" s="29" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G146" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H146" s="40">
         <v>44327</v>
@@ -33416,19 +33421,19 @@
         <v>31</v>
       </c>
       <c r="B148" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C148" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D148" s="8">
         <v>3</v>
       </c>
       <c r="E148" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F148" s="28" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G148" s="10" t="s">
         <v>23</v>
@@ -34459,19 +34464,19 @@
         <v>31</v>
       </c>
       <c r="B149" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C149" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D149" s="8">
         <v>3</v>
       </c>
       <c r="E149" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F149" s="28" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G149" s="10" t="s">
         <v>24</v>
@@ -35502,19 +35507,19 @@
         <v>31</v>
       </c>
       <c r="B150" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C150" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D150" s="8">
         <v>3</v>
       </c>
       <c r="E150" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F150" s="28" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G150" s="10" t="s">
         <v>25</v>
@@ -36545,19 +36550,19 @@
         <v>31</v>
       </c>
       <c r="B151" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C151" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D151" s="8">
         <v>3</v>
       </c>
       <c r="E151" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F151" s="28" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G151" s="10" t="s">
         <v>26</v>
@@ -37588,19 +37593,19 @@
         <v>31</v>
       </c>
       <c r="B152" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C152" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D152" s="8">
         <v>3</v>
       </c>
       <c r="E152" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F152" s="28" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G152" s="10" t="s">
         <v>27</v>
@@ -38632,19 +38637,19 @@
         <v>31</v>
       </c>
       <c r="B153" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C153" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D153" s="8">
         <v>3</v>
       </c>
       <c r="E153" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F153" s="28" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G153" s="10" t="s">
         <v>28</v>
@@ -39676,19 +39681,19 @@
         <v>31</v>
       </c>
       <c r="B154" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C154" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D154" s="14">
         <v>3</v>
       </c>
       <c r="E154" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F154" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G154" s="14" t="s">
         <v>29</v>
@@ -39697,7 +39702,7 @@
         <v>35</v>
       </c>
       <c r="I154" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J154" s="10"/>
       <c r="K154"/>
@@ -41747,85 +41752,85 @@
     </row>
     <row r="156" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A156" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B156" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C156" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D156" s="8">
         <v>3</v>
       </c>
       <c r="E156" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F156" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G156" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H156" s="47">
         <v>601.7722</v>
       </c>
       <c r="I156" s="31" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J156" s="10"/>
     </row>
     <row r="157" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A157" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B157" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C157" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D157" s="8">
         <v>3</v>
       </c>
       <c r="E157" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F157" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G157" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H157" s="47">
         <v>2.8800530000000002</v>
       </c>
       <c r="I157" s="31" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J157" s="10"/>
     </row>
     <row r="158" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A158" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B158" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C158" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D158" s="8">
         <v>3</v>
       </c>
       <c r="E158" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F158" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G158" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H158" s="47">
         <v>-1095.03</v>
@@ -41835,25 +41840,25 @@
     </row>
     <row r="159" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A159" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B159" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C159" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D159" s="8">
         <v>3</v>
       </c>
       <c r="E159" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F159" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G159" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H159" s="47">
         <v>2.7113000000000002E-2</v>
@@ -41863,25 +41868,25 @@
     </row>
     <row r="160" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A160" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B160" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C160" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D160" s="8">
         <v>3</v>
       </c>
       <c r="E160" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F160" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G160" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H160" s="47">
         <v>0</v>
@@ -41891,25 +41896,25 @@
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B161" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C161" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D161" s="8">
         <v>3</v>
       </c>
       <c r="E161" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F161" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G161" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H161" s="47">
         <v>0</v>
@@ -41921,55 +41926,55 @@
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B162" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C162" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D162" s="8">
         <v>3</v>
       </c>
       <c r="E162" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F162" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G162" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H162" s="47">
         <v>-0.223</v>
       </c>
       <c r="I162" s="20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J162" s="10"/>
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B163" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C163" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D163" s="8">
         <v>3</v>
       </c>
       <c r="E163" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F163" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G163" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H163" s="47">
         <v>1</v>
@@ -41981,25 +41986,25 @@
     </row>
     <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B164" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C164" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D164" s="8">
         <v>3</v>
       </c>
       <c r="E164" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F164" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G164" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H164" s="47">
         <v>27.755389999999998</v>
@@ -42009,25 +42014,25 @@
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B165" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C165" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D165" s="8">
         <v>3</v>
       </c>
       <c r="E165" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F165" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G165" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H165" s="47">
         <v>0.52579799999999999</v>
@@ -42037,25 +42042,25 @@
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B166" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C166" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D166" s="8">
         <v>3</v>
       </c>
       <c r="E166" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F166" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G166" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H166" s="47">
         <v>19.667739999999998</v>
@@ -42065,25 +42070,25 @@
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B167" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C167" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D167" s="8">
         <v>3</v>
       </c>
       <c r="E167" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F167" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G167" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H167" s="47">
         <v>34.446179999999998</v>
@@ -42093,25 +42098,25 @@
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B168" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C168" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D168" s="8">
         <v>3</v>
       </c>
       <c r="E168" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F168" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G168" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H168" s="47">
         <v>5.7845329999999997</v>
@@ -42121,25 +42126,25 @@
     </row>
     <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B169" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C169" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D169" s="8">
         <v>3</v>
       </c>
       <c r="E169" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F169" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G169" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H169" s="47">
         <v>-3990.6190000000001</v>
@@ -42149,25 +42154,25 @@
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B170" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C170" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D170" s="8">
         <v>3</v>
       </c>
       <c r="E170" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F170" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G170" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H170" s="47">
         <v>-11590.4</v>
@@ -42177,25 +42182,25 @@
     </row>
     <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B171" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C171" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D171" s="8">
         <v>3</v>
       </c>
       <c r="E171" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F171" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G171" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H171" s="47">
         <v>0</v>
@@ -42205,25 +42210,25 @@
     </row>
     <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B172" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C172" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D172" s="8">
         <v>3</v>
       </c>
       <c r="E172" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F172" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G172" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H172" s="47">
         <v>8388.6</v>
@@ -42233,25 +42238,25 @@
     </row>
     <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B173" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C173" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D173" s="8">
         <v>3</v>
       </c>
       <c r="E173" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F173" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G173" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H173" s="47">
         <v>125829.1</v>
@@ -42273,19 +42278,19 @@
     </row>
     <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B175" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C175" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D175" s="8">
         <v>3</v>
       </c>
       <c r="E175" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F175" s="28">
         <v>8158</v>
@@ -42301,19 +42306,19 @@
     </row>
     <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B176" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C176" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D176" s="8">
         <v>3</v>
       </c>
       <c r="E176" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F176" s="28">
         <v>8158</v>
@@ -42341,19 +42346,19 @@
     </row>
     <row r="178" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A178" s="23" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B178" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C178" s="33" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D178" s="19">
         <v>3</v>
       </c>
       <c r="E178" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F178" s="23">
         <v>55076</v>
@@ -43426,22 +43431,22 @@
     </row>
     <row r="183" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A183" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B183" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C183" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D183" s="8">
         <v>3</v>
       </c>
       <c r="E183" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F183" s="13" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G183" s="10"/>
       <c r="I183" s="8" t="s">
@@ -43451,22 +43456,22 @@
     </row>
     <row r="184" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A184" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B184" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C184" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D184" s="8">
         <v>3</v>
       </c>
       <c r="E184" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F184" s="13" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G184" s="10"/>
       <c r="I184" s="8" t="s">
@@ -43487,22 +43492,22 @@
     </row>
     <row r="186" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A186" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B186" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C186" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D186" s="8">
         <v>3</v>
       </c>
       <c r="E186" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F186" s="13" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G186" s="10"/>
       <c r="I186" s="8" t="s">
@@ -43512,22 +43517,22 @@
     </row>
     <row r="187" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A187" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B187" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C187" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D187" s="8">
         <v>3</v>
       </c>
       <c r="E187" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F187" s="13" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G187" s="10"/>
       <c r="I187" s="8" t="s">
@@ -43537,22 +43542,22 @@
     </row>
     <row r="188" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A188" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B188" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C188" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D188" s="8">
         <v>3</v>
       </c>
       <c r="E188" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F188" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I188" s="8" t="s">
         <v>17</v>
@@ -43561,22 +43566,22 @@
     </row>
     <row r="189" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A189" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B189" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C189" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D189" s="8">
         <v>3</v>
       </c>
       <c r="E189" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F189" s="13" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I189" s="8" t="s">
         <v>17</v>

</xml_diff>